<commit_message>
Fix input for No NARA Match
Align with actual output from merge_format_reports.py: NARA Format Name and Risk Level are "No Match", NARA PRONOM URL and Proposed Preservation Plan are blank (np.NaN), and NARA Match Type is No NARA Match.
</commit_message>
<xml_diff>
--- a/tests/department_reports/check_arguments/archive_formats_by_aip_2021-08.xlsx
+++ b/tests/department_reports/check_arguments/archive_formats_by_aip_2021-08.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amhan\Documents\GitHub\format-report\tests\department_reports\check_arguments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E3235F2-A0C6-467D-A769-CA8C929829C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A84FA26-D7CF-4A13-9D73-AE13033F4223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31530" yWindow="660" windowWidth="19425" windowHeight="15225"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="22245" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="archive_formats_by_aip_2021-08" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="68">
   <si>
     <t>Group</t>
   </si>
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1063,10 +1063,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:P1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1207,14 +1209,8 @@
       <c r="L3" t="s">
         <v>38</v>
       </c>
-      <c r="M3" t="s">
-        <v>25</v>
-      </c>
       <c r="N3" t="s">
         <v>38</v>
-      </c>
-      <c r="O3" t="s">
-        <v>25</v>
       </c>
       <c r="P3" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Replace in department report test csvs
</commit_message>
<xml_diff>
--- a/tests/department_reports/check_arguments/archive_formats_by_aip_2021-08.xlsx
+++ b/tests/department_reports/check_arguments/archive_formats_by_aip_2021-08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amhan\Documents\GitHub\format-report\tests\department_reports\check_arguments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A84FA26-D7CF-4A13-9D73-AE13033F4223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DE0FAE-DE2F-4C2E-A15B-4EFE6650A72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="22245" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="archive_formats_by_aip_2021-08" sheetId="1" r:id="rId1"/>
@@ -31,42 +31,6 @@
     <t>AIP</t>
   </si>
   <si>
-    <t>Format Type</t>
-  </si>
-  <si>
-    <t>Format Standardized Name</t>
-  </si>
-  <si>
-    <t>Format Identification</t>
-  </si>
-  <si>
-    <t>Format Name</t>
-  </si>
-  <si>
-    <t>Format Version</t>
-  </si>
-  <si>
-    <t>Registry Name</t>
-  </si>
-  <si>
-    <t>Registry Key</t>
-  </si>
-  <si>
-    <t>Format Note</t>
-  </si>
-  <si>
-    <t>NARA_Format Name</t>
-  </si>
-  <si>
-    <t>NARA_PRONOM URL</t>
-  </si>
-  <si>
-    <t>NARA_Risk Level</t>
-  </si>
-  <si>
-    <t>NARA_Proposed Preservation Plan</t>
-  </si>
-  <si>
     <t>NARA_Match_Type</t>
   </si>
   <si>
@@ -224,6 +188,42 @@
   </si>
   <si>
     <t>WARC|NO VALUE|NO VALUE</t>
+  </si>
+  <si>
+    <t>Format_Type</t>
+  </si>
+  <si>
+    <t>Format_Standardized_Name</t>
+  </si>
+  <si>
+    <t>Format_Identification</t>
+  </si>
+  <si>
+    <t>Format_Name</t>
+  </si>
+  <si>
+    <t>Format_Version</t>
+  </si>
+  <si>
+    <t>Registry_Name</t>
+  </si>
+  <si>
+    <t>Registry_Key</t>
+  </si>
+  <si>
+    <t>Format_Note</t>
+  </si>
+  <si>
+    <t>NARA_Format_Name</t>
+  </si>
+  <si>
+    <t>NARA_PRONOM_URL</t>
+  </si>
+  <si>
+    <t>NARA_Risk_Level</t>
+  </si>
+  <si>
+    <t>NARA_Proposed_Preservation_Plan</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:P1"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,487 +1083,487 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H2">
         <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="N2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="O2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="P2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="N3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="P3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H4">
         <v>1.01</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="L4" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="M4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="N4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="O4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="P4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H5">
         <v>1.01</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="J5" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="L5" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="M5" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="N5" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="O5" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="P5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="L6" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="M6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N6" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="O6" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="P6" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="K7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="L7" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="M7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N7" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="O7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="P7" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="J8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="K8" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="L8" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="M8" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N8" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="O8" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="P8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="H9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="K9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="L9" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="M9" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N9" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="O9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="P9" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="J10" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="K10" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="L10" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="M10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N10" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="O10" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="P10" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>